<commit_message>
project_pred adjusted, center crop sample error fixed
</commit_message>
<xml_diff>
--- a/yolol__gruber_test.xlsx
+++ b/yolol__gruber_test.xlsx
@@ -622,109 +622,109 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.050734351497134</v>
+        <v>3.792825088367897</v>
       </c>
       <c r="C2" t="n">
-        <v>1.632781158778489</v>
+        <v>1.546691642182422</v>
       </c>
       <c r="D2" t="n">
-        <v>3.960083214968827</v>
+        <v>1.688688498587012</v>
       </c>
       <c r="E2" t="n">
-        <v>1.099133389296103</v>
+        <v>1.081516395373035</v>
       </c>
       <c r="F2" t="n">
-        <v>5.835817614396826</v>
+        <v>1.271113164724866</v>
       </c>
       <c r="G2" t="n">
-        <v>3.811410138723014</v>
+        <v>1.862179354179809</v>
       </c>
       <c r="H2" t="n">
-        <v>3.573698318583399</v>
+        <v>4.217308298119121</v>
       </c>
       <c r="I2" t="n">
-        <v>2.457668201482187</v>
+        <v>2.177799723649859</v>
       </c>
       <c r="J2" t="n">
-        <v>2.567944018181267</v>
+        <v>1.94967491048222</v>
       </c>
       <c r="K2" t="n">
-        <v>0.456155431461593</v>
+        <v>1.158644663925531</v>
       </c>
       <c r="L2" t="n">
-        <v>1.963715440807575</v>
+        <v>1.051738910727824</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8822398406785474</v>
+        <v>1.344899113284217</v>
       </c>
       <c r="N2" t="n">
-        <v>2.39387169005596</v>
+        <v>1.043849219676489</v>
       </c>
       <c r="O2" t="n">
-        <v>1.184580139505974</v>
+        <v>1.05317222826534</v>
       </c>
       <c r="P2" t="n">
-        <v>1.379198488737113</v>
+        <v>0.8505002423756096</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.369998518942603</v>
+        <v>0.9358936184630279</v>
       </c>
       <c r="R2" t="n">
-        <v>1.57835448751356</v>
+        <v>1.106075010245341</v>
       </c>
       <c r="S2" t="n">
-        <v>2.176588801104486</v>
+        <v>1.275889375499644</v>
       </c>
       <c r="T2" t="n">
-        <v>0.5172897253382702</v>
+        <v>1.929619331149395</v>
       </c>
       <c r="U2" t="n">
-        <v>1.569830002170365</v>
+        <v>1.600206971442398</v>
       </c>
       <c r="V2" t="n">
-        <v>3.13107287545438</v>
+        <v>1.301856881026457</v>
       </c>
       <c r="W2" t="n">
-        <v>1.759897264897398</v>
+        <v>1.323910226206807</v>
       </c>
       <c r="X2" t="n">
-        <v>1.891821610616349</v>
+        <v>1.172471701078861</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.657376019225181</v>
+        <v>1.351735241609772</v>
       </c>
       <c r="Z2" t="n">
-        <v>2.492171309610772</v>
+        <v>1.406662577814643</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.808208828190468</v>
+        <v>1.880528686459688</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.704468067359343</v>
+        <v>1.777253694197898</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.5846633420948042</v>
+        <v>2.041188729605869</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.543793000693627</v>
+        <v>1.36513940518563</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.8233388966828248</v>
+        <v>1.560409587992492</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.018688085791013</v>
+        <v>1.003201609179825</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.8876450834267424</v>
+        <v>1.473103553624098</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.7877535007765243</v>
+        <v>1.731918962280045</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.458186562239226</v>
+        <v>7.390936627678586</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.159400541913642</v>
+        <v>2.081786204327535</v>
       </c>
     </row>
     <row r="3">
@@ -733,41 +733,111 @@
           <t>SD</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>5.57554810382968</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9616568858773247</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.30671255003566</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6689411156364747</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8389173022727757</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9154935107345173</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4.140016614340619</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.301037697724458</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.233914165336793</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5353524692443765</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4831433054144341</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.5628273149101107</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.4147661438194007</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.5130690958340587</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.3158494005154383</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.5462863584759837</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.5903789050660904</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.6173073900047488</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1.044443586791306</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.851910146715721</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.6388790428753343</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.5748645361840525</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.4961483590010816</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.6115925526840317</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.8800274962732321</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1.219838824567253</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.9519792161616931</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1.078894259070486</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.7474179547294174</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.8634578096904488</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.4890578176541391</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1.000423185388284</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1.298616981540407</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>9.850804531664439</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1.212763345597955</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -776,109 +846,109 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.050734351497134</v>
+        <v>6.785091908209915</v>
       </c>
       <c r="C4" t="n">
-        <v>1.632781158778489</v>
+        <v>1.830652960054959</v>
       </c>
       <c r="D4" t="n">
-        <v>3.960083214968827</v>
+        <v>2.149978415893389</v>
       </c>
       <c r="E4" t="n">
-        <v>1.099133389296103</v>
+        <v>1.268585576322448</v>
       </c>
       <c r="F4" t="n">
-        <v>5.835817614396826</v>
+        <v>1.518935107483683</v>
       </c>
       <c r="G4" t="n">
-        <v>3.811410138723014</v>
+        <v>2.411321500357255</v>
       </c>
       <c r="H4" t="n">
-        <v>3.573698318583399</v>
+        <v>7.96816516688512</v>
       </c>
       <c r="I4" t="n">
-        <v>2.457668201482187</v>
+        <v>2.562365772017433</v>
       </c>
       <c r="J4" t="n">
-        <v>2.567944018181267</v>
+        <v>2.319518689017587</v>
       </c>
       <c r="K4" t="n">
-        <v>0.456155431461593</v>
+        <v>1.289748811020303</v>
       </c>
       <c r="L4" t="n">
-        <v>1.963715440807575</v>
+        <v>1.157403209735369</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8822398406785474</v>
+        <v>1.484237851259173</v>
       </c>
       <c r="N4" t="n">
-        <v>2.39387169005596</v>
+        <v>1.126065568381799</v>
       </c>
       <c r="O4" t="n">
-        <v>1.184580139505974</v>
+        <v>1.17149973943205</v>
       </c>
       <c r="P4" t="n">
-        <v>1.379198488737113</v>
+        <v>0.9072549289405555</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.369998518942603</v>
+        <v>1.08366307057903</v>
       </c>
       <c r="R4" t="n">
-        <v>1.57835448751356</v>
+        <v>1.25377397478025</v>
       </c>
       <c r="S4" t="n">
-        <v>2.176588801104486</v>
+        <v>1.427681710736513</v>
       </c>
       <c r="T4" t="n">
-        <v>0.5172897253382702</v>
+        <v>2.194149759960548</v>
       </c>
       <c r="U4" t="n">
-        <v>1.569830002170365</v>
+        <v>1.841220233773073</v>
       </c>
       <c r="V4" t="n">
-        <v>3.13107287545438</v>
+        <v>1.452728115631185</v>
       </c>
       <c r="W4" t="n">
-        <v>1.759897264897398</v>
+        <v>1.443332089997678</v>
       </c>
       <c r="X4" t="n">
-        <v>1.891821610616349</v>
+        <v>1.273127285062347</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.657376019225181</v>
+        <v>1.483655490303729</v>
       </c>
       <c r="Z4" t="n">
-        <v>2.492171309610772</v>
+        <v>1.659261282023139</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.808208828190468</v>
+        <v>2.288442110368584</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.704468067359343</v>
+        <v>2.020240742238044</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.5846633420948042</v>
+        <v>2.350418343437572</v>
       </c>
       <c r="AD4" t="n">
-        <v>2.543793000693627</v>
+        <v>1.559614109057333</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.8233388966828248</v>
+        <v>1.78337810668807</v>
       </c>
       <c r="AF4" t="n">
-        <v>2.018688085791013</v>
+        <v>1.116060490148101</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.8876450834267424</v>
+        <v>1.780696669722945</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.7877535007765243</v>
+        <v>2.164705374098356</v>
       </c>
       <c r="AI4" t="n">
-        <v>1.458186562239226</v>
+        <v>13.14380415315603</v>
       </c>
       <c r="AJ4" t="n">
-        <v>1.159400541913642</v>
+        <v>2.42649567819505</v>
       </c>
     </row>
     <row r="5">
@@ -888,109 +958,109 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.2363636363636364</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.7592592592592593</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0.9122807017543859</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.5192307692307693</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.5740740740740741</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>0.9107142857142857</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.8269230769230769</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>0.7551020408163265</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="W5" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>0.9464285714285714</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>0.8392857142857143</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="AA5" t="n">
-        <v>1</v>
+        <v>0.673469387755102</v>
       </c>
       <c r="AB5" t="n">
-        <v>1</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AD5" t="n">
-        <v>0</v>
+        <v>0.8545454545454545</v>
       </c>
       <c r="AE5" t="n">
-        <v>1</v>
+        <v>0.7321428571428571</v>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>0.9464285714285714</v>
       </c>
       <c r="AG5" t="n">
-        <v>1</v>
+        <v>0.7678571428571429</v>
       </c>
       <c r="AH5" t="n">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AI5" t="n">
-        <v>1</v>
+        <v>0.3478260869565217</v>
       </c>
       <c r="AJ5" t="n">
-        <v>1</v>
+        <v>0.5660377358490566</v>
       </c>
     </row>
     <row r="6">
@@ -1000,40 +1070,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.3818181818181818</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="N6" t="n">
         <v>1</v>
@@ -1045,64 +1115,64 @@
         <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>0.7678571428571429</v>
       </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>0.9272727272727272</v>
       </c>
       <c r="W6" t="n">
-        <v>1</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="X6" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="AA6" t="n">
-        <v>1</v>
+        <v>0.7551020408163265</v>
       </c>
       <c r="AB6" t="n">
-        <v>1</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="AC6" t="n">
-        <v>1</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
+        <v>0.8909090909090909</v>
       </c>
       <c r="AE6" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="AF6" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="AG6" t="n">
-        <v>1</v>
+        <v>0.8392857142857143</v>
       </c>
       <c r="AH6" t="n">
-        <v>1</v>
+        <v>0.8035714285714286</v>
       </c>
       <c r="AI6" t="n">
-        <v>1</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1</v>
+        <v>0.6981132075471698</v>
       </c>
     </row>
     <row r="7">
@@ -1112,31 +1182,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.9074074074074074</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0.7115384615384616</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -1166,16 +1236,16 @@
         <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="U7" t="n">
-        <v>1</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>0.9636363636363636</v>
       </c>
       <c r="W7" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="X7" t="n">
         <v>1</v>
@@ -1184,37 +1254,37 @@
         <v>1</v>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AA7" t="n">
-        <v>1</v>
+        <v>0.8367346938775511</v>
       </c>
       <c r="AB7" t="n">
-        <v>1</v>
+        <v>0.8545454545454545</v>
       </c>
       <c r="AC7" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="AD7" t="n">
-        <v>1</v>
+        <v>0.9454545454545454</v>
       </c>
       <c r="AE7" t="n">
-        <v>1</v>
+        <v>0.9464285714285714</v>
       </c>
       <c r="AF7" t="n">
         <v>1</v>
       </c>
       <c r="AG7" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="AH7" t="n">
-        <v>1</v>
+        <v>0.8392857142857143</v>
       </c>
       <c r="AI7" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AJ7" t="n">
-        <v>1</v>
+        <v>0.7169811320754716</v>
       </c>
     </row>
     <row r="8">
@@ -1224,31 +1294,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.7818181818181819</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.9824561403508771</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0.9038461538461539</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="K8" t="n">
         <v>1</v>
@@ -1278,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="U8" t="n">
-        <v>1</v>
+        <v>0.9795918367346939</v>
       </c>
       <c r="V8" t="n">
         <v>1</v>
@@ -1299,34 +1369,34 @@
         <v>1</v>
       </c>
       <c r="AA8" t="n">
-        <v>1</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="AB8" t="n">
-        <v>1</v>
+        <v>0.9636363636363636</v>
       </c>
       <c r="AC8" t="n">
-        <v>1</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
       </c>
       <c r="AE8" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="AF8" t="n">
         <v>1</v>
       </c>
       <c r="AG8" t="n">
-        <v>1</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="AH8" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AI8" t="n">
-        <v>1</v>
+        <v>0.6521739130434783</v>
       </c>
       <c r="AJ8" t="n">
-        <v>1</v>
+        <v>0.9245283018867925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>